<commit_message>
- updated bom and place
</commit_message>
<xml_diff>
--- a/hardware/raspi-hat/bom.xlsx
+++ b/hardware/raspi-hat/bom.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$23</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$26</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="94">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -110,7 +110,7 @@
     <t xml:space="preserve">1u</t>
   </si>
   <si>
-    <t xml:space="preserve">C5,C6,C7,C8,C10</t>
+    <t xml:space="preserve">C5,C6,C7,C10</t>
   </si>
   <si>
     <t xml:space="preserve">C_1206_3216Metric</t>
@@ -119,6 +119,12 @@
     <t xml:space="preserve">C1848</t>
   </si>
   <si>
+    <t xml:space="preserve">C8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C15849</t>
+  </si>
+  <si>
     <t xml:space="preserve">47u</t>
   </si>
   <si>
@@ -191,6 +197,18 @@
     <t xml:space="preserve">C5355286</t>
   </si>
   <si>
+    <t xml:space="preserve">USB_C_Receptacle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB_C_Receptacle_Molex_105450-0101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C134092</t>
+  </si>
+  <si>
     <t xml:space="preserve">15u</t>
   </si>
   <si>
@@ -296,6 +314,12 @@
     <t xml:space="preserve">C48484</t>
   </si>
   <si>
+    <t xml:space="preserve">TH1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C13564</t>
+  </si>
+  <si>
     <t xml:space="preserve">STSPIN32G4</t>
   </si>
   <si>
@@ -318,12 +342,6 @@
   </si>
   <si>
     <t xml:space="preserve">C9009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TH1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C13564</t>
   </si>
 </sst>
 </file>
@@ -434,7 +452,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -455,7 +473,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -463,7 +481,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -575,13 +597,13 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="21.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="51.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.41"/>
   </cols>
@@ -655,160 +677,160 @@
       <c r="D5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="0"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" s="6" customFormat="true" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" s="6" customFormat="true" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="0"/>
-    </row>
-    <row r="7" s="6" customFormat="true" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" s="6" customFormat="true" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="0"/>
-    </row>
-    <row r="8" s="6" customFormat="true" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="0"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="D9" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="D10" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="D11" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="D12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="2" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="C13" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="D14" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="D15" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>60</v>
@@ -822,7 +844,7 @@
         <v>62</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>63</v>
@@ -836,35 +858,35 @@
         <v>65</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="7" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="B19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="C19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>73</v>
@@ -878,52 +900,80 @@
         <v>75</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="D23" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="5" t="s">
+      <c r="B25" s="2" t="s">
         <v>87</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -957,7 +1007,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:D23"/>
+  <autoFilter ref="A1:D26"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>